<commit_message>
change some excel file
</commit_message>
<xml_diff>
--- a/真值表自动生成表达式.xlsx
+++ b/真值表自动生成表达式.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loyio/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loyio/computer-hardware-design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B2D5CEA-DEB8-B143-9181-BC6FD00C9968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942CAD9-7479-1B43-940E-FB3ABAA4EDC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="组合逻辑真值表" sheetId="3" r:id="rId1"/>
@@ -1176,9 +1176,9 @@
   </sheetPr>
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1296,14 +1296,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:24" ht="16">
+      <c r="A3" s="19">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0</v>
+      </c>
+      <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -1311,33 +1317,45 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
-      <c r="M3" s="20">
-        <v>1</v>
-      </c>
-      <c r="N3" s="19"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="19">
+        <v>1</v>
+      </c>
       <c r="O3" s="19">
         <v>1</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
+      <c r="P3" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>1</v>
+      </c>
+      <c r="R3" s="19">
+        <v>1</v>
+      </c>
+      <c r="S3" s="19">
+        <v>1</v>
+      </c>
       <c r="T3" s="19"/>
       <c r="U3" s="19"/>
       <c r="V3" s="19"/>
       <c r="W3" s="19"/>
       <c r="X3" s="19"/>
     </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+    <row r="4" spans="1:24" ht="16">
+      <c r="A4" s="21">
+        <v>0</v>
+      </c>
+      <c r="B4" s="21">
+        <v>0</v>
+      </c>
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
       <c r="D4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="21">
-        <v>0</v>
-      </c>
+      <c r="E4" s="21"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -1347,20 +1365,22 @@
       <c r="L4" s="21"/>
       <c r="M4" s="22"/>
       <c r="N4" s="21"/>
-      <c r="O4" s="21">
-        <v>1</v>
-      </c>
-      <c r="P4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21">
+        <v>1</v>
+      </c>
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
+      <c r="S4" s="21">
+        <v>1</v>
+      </c>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" ht="16">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19">
@@ -1369,9 +1389,7 @@
       <c r="D5" s="19">
         <v>0</v>
       </c>
-      <c r="E5" s="19">
-        <v>0</v>
-      </c>
+      <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -1382,13 +1400,19 @@
       <c r="M5" s="23">
         <v>1</v>
       </c>
-      <c r="N5" s="24">
-        <v>1</v>
-      </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24">
+        <v>1</v>
+      </c>
+      <c r="P5" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="24">
+        <v>1</v>
+      </c>
+      <c r="R5" s="24">
+        <v>1</v>
+      </c>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
@@ -1396,7 +1420,7 @@
       <c r="W5" s="24"/>
       <c r="X5" s="24"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="16">
       <c r="A6" s="21"/>
       <c r="B6" s="21">
         <v>1</v>
@@ -1407,9 +1431,7 @@
       <c r="D6" s="21">
         <v>0</v>
       </c>
-      <c r="E6" s="21">
-        <v>0</v>
-      </c>
+      <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -1417,22 +1439,30 @@
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="21">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
+      <c r="M6" s="22">
+        <v>1</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21">
+        <v>1</v>
+      </c>
+      <c r="P6" s="21">
+        <v>1</v>
+      </c>
       <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="R6" s="21">
+        <v>1</v>
+      </c>
+      <c r="S6" s="21">
+        <v>1</v>
+      </c>
       <c r="T6" s="21"/>
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" ht="16">
       <c r="A7" s="19">
         <v>1</v>
       </c>
@@ -1445,9 +1475,7 @@
       <c r="D7" s="19">
         <v>0</v>
       </c>
-      <c r="E7" s="19">
-        <v>0</v>
-      </c>
+      <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -1458,19 +1486,25 @@
       <c r="M7" s="23">
         <v>1</v>
       </c>
-      <c r="N7" s="24"/>
+      <c r="N7" s="24">
+        <v>1</v>
+      </c>
       <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
+      <c r="P7" s="24">
+        <v>1</v>
+      </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
+      <c r="S7" s="24">
+        <v>1</v>
+      </c>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
       <c r="X7" s="24"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" ht="16">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1483,13 +1517,23 @@
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="M8" s="22">
+        <v>1</v>
+      </c>
+      <c r="N8" s="21">
+        <v>1</v>
+      </c>
+      <c r="O8" s="21">
+        <v>1</v>
+      </c>
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
+      <c r="R8" s="21">
+        <v>1</v>
+      </c>
+      <c r="S8" s="21">
+        <v>1</v>
+      </c>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
       <c r="V8" s="21"/>
@@ -1509,13 +1553,25 @@
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
+      <c r="M9" s="23">
+        <v>1</v>
+      </c>
+      <c r="N9" s="24">
+        <v>1</v>
+      </c>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
       <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
+      <c r="Q9" s="24">
+        <v>1</v>
+      </c>
+      <c r="R9" s="24">
+        <v>1</v>
+      </c>
+      <c r="S9" s="24">
+        <v>1</v>
+      </c>
       <c r="T9" s="24"/>
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
@@ -1537,11 +1593,17 @@
       <c r="L10" s="21"/>
       <c r="M10" s="22"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
+      <c r="O10" s="21">
+        <v>1</v>
+      </c>
+      <c r="P10" s="21">
+        <v>1</v>
+      </c>
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
+      <c r="S10" s="21">
+        <v>1</v>
+      </c>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
       <c r="V10" s="21"/>
@@ -1561,13 +1623,27 @@
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
+      <c r="M11" s="23">
+        <v>1</v>
+      </c>
+      <c r="N11" s="24">
+        <v>1</v>
+      </c>
+      <c r="O11" s="24">
+        <v>1</v>
+      </c>
+      <c r="P11" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>1</v>
+      </c>
+      <c r="R11" s="24">
+        <v>1</v>
+      </c>
+      <c r="S11" s="24">
+        <v>1</v>
+      </c>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
@@ -1587,13 +1663,25 @@
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
+      <c r="M12" s="22">
+        <v>1</v>
+      </c>
+      <c r="N12" s="21">
+        <v>1</v>
+      </c>
+      <c r="O12" s="21">
+        <v>1</v>
+      </c>
+      <c r="P12" s="21">
+        <v>1</v>
+      </c>
       <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
+      <c r="R12" s="21">
+        <v>1</v>
+      </c>
+      <c r="S12" s="21">
+        <v>1</v>
+      </c>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
@@ -1613,13 +1701,25 @@
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="M13" s="23">
+        <v>1</v>
+      </c>
+      <c r="N13" s="24">
+        <v>1</v>
+      </c>
+      <c r="O13" s="24">
+        <v>1</v>
+      </c>
+      <c r="P13" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>1</v>
+      </c>
       <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
+      <c r="S13" s="24">
+        <v>1</v>
+      </c>
       <c r="T13" s="24"/>
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
@@ -1639,13 +1739,23 @@
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="21"/>
+      <c r="M14" s="22">
+        <v>1</v>
+      </c>
+      <c r="N14" s="21">
+        <v>1</v>
+      </c>
       <c r="O14" s="21"/>
       <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
+      <c r="Q14" s="21">
+        <v>1</v>
+      </c>
+      <c r="R14" s="21">
+        <v>1</v>
+      </c>
+      <c r="S14" s="21">
+        <v>1</v>
+      </c>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
       <c r="V14" s="21"/>
@@ -1666,11 +1776,19 @@
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="23"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
+      <c r="N15" s="24">
+        <v>1</v>
+      </c>
+      <c r="O15" s="24">
+        <v>1</v>
+      </c>
       <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="Q15" s="24">
+        <v>1</v>
+      </c>
+      <c r="R15" s="24">
+        <v>1</v>
+      </c>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
@@ -1691,13 +1809,23 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
-      <c r="M16" s="22"/>
+      <c r="M16" s="22">
+        <v>1</v>
+      </c>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
+      <c r="P16" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>1</v>
+      </c>
+      <c r="R16" s="21">
+        <v>1</v>
+      </c>
+      <c r="S16" s="21">
+        <v>1</v>
+      </c>
       <c r="T16" s="21"/>
       <c r="U16" s="21"/>
       <c r="V16" s="21"/>
@@ -1717,12 +1845,22 @@
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
+      <c r="M17" s="23">
+        <v>1</v>
+      </c>
+      <c r="N17" s="24">
+        <v>1</v>
+      </c>
+      <c r="O17" s="24">
+        <v>1</v>
+      </c>
       <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
+      <c r="Q17" s="24">
+        <v>1</v>
+      </c>
+      <c r="R17" s="24">
+        <v>1</v>
+      </c>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="24"/>
@@ -1743,11 +1881,19 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
+      <c r="M18" s="22">
+        <v>1</v>
+      </c>
+      <c r="N18" s="21">
+        <v>1</v>
+      </c>
+      <c r="O18" s="21">
+        <v>1</v>
+      </c>
       <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
+      <c r="Q18" s="21">
+        <v>1</v>
+      </c>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="21"/>
@@ -2184,8 +2330,8 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="400" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
@@ -2303,23 +2449,23 @@
     <row r="2" spans="1:25" ht="16" thickTop="1">
       <c r="A2" s="16" t="str">
         <f>IF(组合逻辑真值表!A3&lt;&gt;"",IF(组合逻辑真值表!A3=1,组合逻辑真值表!A$2&amp;"&amp;",IF(组合逻辑真值表!A3=0,"~"&amp;组合逻辑真值表!A$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In1&amp;</v>
       </c>
       <c r="B2" s="16" t="str">
         <f>IF(组合逻辑真值表!B3&lt;&gt;"",IF(组合逻辑真值表!B3=1,组合逻辑真值表!B$2&amp;"&amp;",IF(组合逻辑真值表!B3=0,"~"&amp;组合逻辑真值表!B$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In2&amp;</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>IF(组合逻辑真值表!C3&lt;&gt;"",IF(组合逻辑真值表!C3=1,组合逻辑真值表!C$2&amp;"&amp;",IF(组合逻辑真值表!C3=0,"~"&amp;组合逻辑真值表!C$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In3&amp;</v>
       </c>
       <c r="D2" s="16" t="str">
         <f>IF(组合逻辑真值表!D3&lt;&gt;"",IF(组合逻辑真值表!D3=1,组合逻辑真值表!D$2&amp;"&amp;",IF(组合逻辑真值表!D3=0,"~"&amp;组合逻辑真值表!D$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In4&amp;</v>
       </c>
       <c r="E2" s="16" t="str">
         <f>IF(组合逻辑真值表!E3&lt;&gt;"",IF(组合逻辑真值表!E3=1,组合逻辑真值表!E$2&amp;"&amp;",IF(组合逻辑真值表!E3=0,"~"&amp;组合逻辑真值表!E$2&amp;"&amp;","")),"")</f>
-        <v>In5&amp;</v>
+        <v/>
       </c>
       <c r="F2" s="16" t="str">
         <f>IF(组合逻辑真值表!F3&lt;&gt;"",IF(组合逻辑真值表!F3=1,组合逻辑真值表!F$2&amp;"&amp;",IF(组合逻辑真值表!F3=0,"~"&amp;组合逻辑真值表!F$2&amp;"&amp;","")),"")</f>
@@ -2351,35 +2497,35 @@
       </c>
       <c r="M2" s="3" t="str">
         <f>IF(LEN(CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2))=0,"",LEFT(CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2),LEN(CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2))-1))</f>
-        <v>In5</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4</v>
       </c>
       <c r="N2" s="4" t="str">
         <f>IF(组合逻辑真值表!M3=1,$M2&amp;"+","")</f>
-        <v>In5+</v>
+        <v/>
       </c>
       <c r="O2" s="4" t="str">
         <f>IF(组合逻辑真值表!N3=1,$M2&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="P2" s="4" t="str">
         <f>IF(组合逻辑真值表!O3=1,$M2&amp;"+","")</f>
-        <v>In5+</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="Q2" s="4" t="str">
         <f>IF(组合逻辑真值表!P3=1,$M2&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="R2" s="4" t="str">
         <f>IF(组合逻辑真值表!Q3=1,$M2&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="S2" s="4" t="str">
         <f>IF(组合逻辑真值表!R3=1,$M2&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="T2" s="4" t="str">
         <f>IF(组合逻辑真值表!S3=1,$M2&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="U2" s="4" t="str">
         <f>IF(组合逻辑真值表!T3=1,$M2&amp;"+","")</f>
@@ -2405,15 +2551,15 @@
     <row r="3" spans="1:25">
       <c r="A3" s="16" t="str">
         <f>IF(组合逻辑真值表!A4&lt;&gt;"",IF(组合逻辑真值表!A4=1,组合逻辑真值表!A$2&amp;"&amp;",IF(组合逻辑真值表!A4=0,"~"&amp;组合逻辑真值表!A$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In1&amp;</v>
       </c>
       <c r="B3" s="16" t="str">
         <f>IF(组合逻辑真值表!B4&lt;&gt;"",IF(组合逻辑真值表!B4=1,组合逻辑真值表!B$2&amp;"&amp;",IF(组合逻辑真值表!B4=0,"~"&amp;组合逻辑真值表!B$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In2&amp;</v>
       </c>
       <c r="C3" s="16" t="str">
         <f>IF(组合逻辑真值表!C4&lt;&gt;"",IF(组合逻辑真值表!C4=1,组合逻辑真值表!C$2&amp;"&amp;",IF(组合逻辑真值表!C4=0,"~"&amp;组合逻辑真值表!C$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~In3&amp;</v>
       </c>
       <c r="D3" s="16" t="str">
         <f>IF(组合逻辑真值表!D4&lt;&gt;"",IF(组合逻辑真值表!D4=1,组合逻辑真值表!D$2&amp;"&amp;",IF(组合逻辑真值表!D4=0,"~"&amp;组合逻辑真值表!D$2&amp;"&amp;","")),"")</f>
@@ -2421,7 +2567,7 @@
       </c>
       <c r="E3" s="16" t="str">
         <f>IF(组合逻辑真值表!E4&lt;&gt;"",IF(组合逻辑真值表!E4=1,组合逻辑真值表!E$2&amp;"&amp;",IF(组合逻辑真值表!E4=0,"~"&amp;组合逻辑真值表!E$2&amp;"&amp;","")),"")</f>
-        <v>~In5&amp;</v>
+        <v/>
       </c>
       <c r="F3" s="16" t="str">
         <f>IF(组合逻辑真值表!F4&lt;&gt;"",IF(组合逻辑真值表!F4=1,组合逻辑真值表!F$2&amp;"&amp;",IF(组合逻辑真值表!F4=0,"~"&amp;组合逻辑真值表!F$2&amp;"&amp;","")),"")</f>
@@ -2453,7 +2599,7 @@
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" ref="M3:M19" si="0">IF(LEN(CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3))=0,"",LEFT(CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3),LEN(CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3))-1))</f>
-        <v>In4&amp;~In5</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;In4</v>
       </c>
       <c r="N3" s="4" t="str">
         <f>IF(组合逻辑真值表!M4=1,$M3&amp;"+","")</f>
@@ -2465,11 +2611,11 @@
       </c>
       <c r="P3" s="4" t="str">
         <f>IF(组合逻辑真值表!O4=1,$M3&amp;"+","")</f>
-        <v>In4&amp;~In5+</v>
+        <v/>
       </c>
       <c r="Q3" s="4" t="str">
         <f>IF(组合逻辑真值表!P4=1,$M3&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;In4+</v>
       </c>
       <c r="R3" s="4" t="str">
         <f>IF(组合逻辑真值表!Q4=1,$M3&amp;"+","")</f>
@@ -2481,7 +2627,7 @@
       </c>
       <c r="T3" s="4" t="str">
         <f>IF(组合逻辑真值表!S4=1,$M3&amp;"+","")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;In4+</v>
       </c>
       <c r="U3" s="4" t="str">
         <f>IF(组合逻辑真值表!T4=1,$M3&amp;"+","")</f>
@@ -2523,7 +2669,7 @@
       </c>
       <c r="E4" s="16" t="str">
         <f>IF(组合逻辑真值表!E5&lt;&gt;"",IF(组合逻辑真值表!E5=1,组合逻辑真值表!E$2&amp;"&amp;",IF(组合逻辑真值表!E5=0,"~"&amp;组合逻辑真值表!E$2&amp;"&amp;","")),"")</f>
-        <v>~In5&amp;</v>
+        <v/>
       </c>
       <c r="F4" s="16" t="str">
         <f>IF(组合逻辑真值表!F5&lt;&gt;"",IF(组合逻辑真值表!F5=1,组合逻辑真值表!F$2&amp;"&amp;",IF(组合逻辑真值表!F5=0,"~"&amp;组合逻辑真值表!F$2&amp;"&amp;","")),"")</f>
@@ -2555,31 +2701,31 @@
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>In3&amp;~In4&amp;~In5</v>
+        <v>In3&amp;~In4</v>
       </c>
       <c r="N4" s="4" t="str">
         <f>IF(组合逻辑真值表!M5=1,$M4&amp;"+","")</f>
-        <v>In3&amp;~In4&amp;~In5+</v>
+        <v>In3&amp;~In4+</v>
       </c>
       <c r="O4" s="4" t="str">
         <f>IF(组合逻辑真值表!N5=1,$M4&amp;"+","")</f>
-        <v>In3&amp;~In4&amp;~In5+</v>
+        <v/>
       </c>
       <c r="P4" s="4" t="str">
         <f>IF(组合逻辑真值表!O5=1,$M4&amp;"+","")</f>
-        <v/>
+        <v>In3&amp;~In4+</v>
       </c>
       <c r="Q4" s="4" t="str">
         <f>IF(组合逻辑真值表!P5=1,$M4&amp;"+","")</f>
-        <v/>
+        <v>In3&amp;~In4+</v>
       </c>
       <c r="R4" s="4" t="str">
         <f>IF(组合逻辑真值表!Q5=1,$M4&amp;"+","")</f>
-        <v/>
+        <v>In3&amp;~In4+</v>
       </c>
       <c r="S4" s="4" t="str">
         <f>IF(组合逻辑真值表!R5=1,$M4&amp;"+","")</f>
-        <v/>
+        <v>In3&amp;~In4+</v>
       </c>
       <c r="T4" s="4" t="str">
         <f>IF(组合逻辑真值表!S5=1,$M4&amp;"+","")</f>
@@ -2625,7 +2771,7 @@
       </c>
       <c r="E5" s="16" t="str">
         <f>IF(组合逻辑真值表!E6&lt;&gt;"",IF(组合逻辑真值表!E6=1,组合逻辑真值表!E$2&amp;"&amp;",IF(组合逻辑真值表!E6=0,"~"&amp;组合逻辑真值表!E$2&amp;"&amp;","")),"")</f>
-        <v>~In5&amp;</v>
+        <v/>
       </c>
       <c r="F5" s="16" t="str">
         <f>IF(组合逻辑真值表!F6&lt;&gt;"",IF(组合逻辑真值表!F6=1,组合逻辑真值表!F$2&amp;"&amp;",IF(组合逻辑真值表!F6=0,"~"&amp;组合逻辑真值表!F$2&amp;"&amp;","")),"")</f>
@@ -2657,23 +2803,23 @@
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>In2&amp;~In3&amp;~In4&amp;~In5</v>
+        <v>In2&amp;~In3&amp;~In4</v>
       </c>
       <c r="N5" s="4" t="str">
         <f>IF(组合逻辑真值表!M6=1,$M5&amp;"+","")</f>
-        <v/>
+        <v>In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="O5" s="4" t="str">
         <f>IF(组合逻辑真值表!N6=1,$M5&amp;"+","")</f>
-        <v>In2&amp;~In3&amp;~In4&amp;~In5+</v>
+        <v/>
       </c>
       <c r="P5" s="4" t="str">
         <f>IF(组合逻辑真值表!O6=1,$M5&amp;"+","")</f>
-        <v/>
+        <v>In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="Q5" s="4" t="str">
         <f>IF(组合逻辑真值表!P6=1,$M5&amp;"+","")</f>
-        <v/>
+        <v>In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="R5" s="4" t="str">
         <f>IF(组合逻辑真值表!Q6=1,$M5&amp;"+","")</f>
@@ -2681,11 +2827,11 @@
       </c>
       <c r="S5" s="4" t="str">
         <f>IF(组合逻辑真值表!R6=1,$M5&amp;"+","")</f>
-        <v/>
+        <v>In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="T5" s="4" t="str">
         <f>IF(组合逻辑真值表!S6=1,$M5&amp;"+","")</f>
-        <v/>
+        <v>In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="U5" s="4" t="str">
         <f>IF(组合逻辑真值表!T6=1,$M5&amp;"+","")</f>
@@ -2727,7 +2873,7 @@
       </c>
       <c r="E6" s="16" t="str">
         <f>IF(组合逻辑真值表!E7&lt;&gt;"",IF(组合逻辑真值表!E7=1,组合逻辑真值表!E$2&amp;"&amp;",IF(组合逻辑真值表!E7=0,"~"&amp;组合逻辑真值表!E$2&amp;"&amp;","")),"")</f>
-        <v>~In5&amp;</v>
+        <v/>
       </c>
       <c r="F6" s="16" t="str">
         <f>IF(组合逻辑真值表!F7&lt;&gt;"",IF(组合逻辑真值表!F7=1,组合逻辑真值表!F$2&amp;"&amp;",IF(组合逻辑真值表!F7=0,"~"&amp;组合逻辑真值表!F$2&amp;"&amp;","")),"")</f>
@@ -2759,15 +2905,15 @@
       </c>
       <c r="M6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>In1&amp;~In2&amp;~In3&amp;~In4&amp;~In5</v>
+        <v>In1&amp;~In2&amp;~In3&amp;~In4</v>
       </c>
       <c r="N6" s="4" t="str">
         <f>IF(组合逻辑真值表!M7=1,$M6&amp;"+","")</f>
-        <v>In1&amp;~In2&amp;~In3&amp;~In4&amp;~In5+</v>
+        <v>In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="O6" s="4" t="str">
         <f>IF(组合逻辑真值表!N7=1,$M6&amp;"+","")</f>
-        <v/>
+        <v>In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="P6" s="4" t="str">
         <f>IF(组合逻辑真值表!O7=1,$M6&amp;"+","")</f>
@@ -2775,7 +2921,7 @@
       </c>
       <c r="Q6" s="4" t="str">
         <f>IF(组合逻辑真值表!P7=1,$M6&amp;"+","")</f>
-        <v/>
+        <v>In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="R6" s="4" t="str">
         <f>IF(组合逻辑真值表!Q7=1,$M6&amp;"+","")</f>
@@ -2787,7 +2933,7 @@
       </c>
       <c r="T6" s="4" t="str">
         <f>IF(组合逻辑真值表!S7=1,$M6&amp;"+","")</f>
-        <v/>
+        <v>In1&amp;~In2&amp;~In3&amp;~In4+</v>
       </c>
       <c r="U6" s="4" t="str">
         <f>IF(组合逻辑真值表!T7=1,$M6&amp;"+","")</f>
@@ -2865,15 +3011,15 @@
       </c>
       <c r="N7" s="4" t="str">
         <f>IF(组合逻辑真值表!M8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O7" s="4" t="str">
         <f>IF(组合逻辑真值表!N8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P7" s="4" t="str">
         <f>IF(组合逻辑真值表!O8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q7" s="4" t="str">
         <f>IF(组合逻辑真值表!P8=1,$M7&amp;"+","")</f>
@@ -2885,11 +3031,11 @@
       </c>
       <c r="S7" s="4" t="str">
         <f>IF(组合逻辑真值表!R8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T7" s="4" t="str">
         <f>IF(组合逻辑真值表!S8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U7" s="4" t="str">
         <f>IF(组合逻辑真值表!T8=1,$M7&amp;"+","")</f>
@@ -2967,15 +3113,15 @@
       </c>
       <c r="N8" s="4" t="str">
         <f>IF(组合逻辑真值表!M9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O8" s="4" t="str">
         <f>IF(组合逻辑真值表!N9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P8" s="4" t="str">
         <f>IF(组合逻辑真值表!O9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q8" s="4" t="str">
         <f>IF(组合逻辑真值表!P9=1,$M8&amp;"+","")</f>
@@ -2983,15 +3129,15 @@
       </c>
       <c r="R8" s="4" t="str">
         <f>IF(组合逻辑真值表!Q9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S8" s="4" t="str">
         <f>IF(组合逻辑真值表!R9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T8" s="4" t="str">
         <f>IF(组合逻辑真值表!S9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U8" s="4" t="str">
         <f>IF(组合逻辑真值表!T9=1,$M8&amp;"+","")</f>
@@ -3077,11 +3223,11 @@
       </c>
       <c r="P9" s="4" t="str">
         <f>IF(组合逻辑真值表!O10=1,$M9&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q9" s="4" t="str">
         <f>IF(组合逻辑真值表!P10=1,$M9&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="R9" s="4" t="str">
         <f>IF(组合逻辑真值表!Q10=1,$M9&amp;"+","")</f>
@@ -3093,7 +3239,7 @@
       </c>
       <c r="T9" s="4" t="str">
         <f>IF(组合逻辑真值表!S10=1,$M9&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U9" s="4" t="str">
         <f>IF(组合逻辑真值表!T10=1,$M9&amp;"+","")</f>
@@ -3171,31 +3317,31 @@
       </c>
       <c r="N10" s="4" t="str">
         <f>IF(组合逻辑真值表!M11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O10" s="4" t="str">
         <f>IF(组合逻辑真值表!N11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P10" s="4" t="str">
         <f>IF(组合逻辑真值表!O11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q10" s="4" t="str">
         <f>IF(组合逻辑真值表!P11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="R10" s="4" t="str">
         <f>IF(组合逻辑真值表!Q11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S10" s="4" t="str">
         <f>IF(组合逻辑真值表!R11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T10" s="4" t="str">
         <f>IF(组合逻辑真值表!S11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U10" s="4" t="str">
         <f>IF(组合逻辑真值表!T11=1,$M10&amp;"+","")</f>
@@ -3273,19 +3419,19 @@
       </c>
       <c r="N11" s="4" t="str">
         <f>IF(组合逻辑真值表!M12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O11" s="4" t="str">
         <f>IF(组合逻辑真值表!N12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P11" s="4" t="str">
         <f>IF(组合逻辑真值表!O12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q11" s="4" t="str">
         <f>IF(组合逻辑真值表!P12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="R11" s="4" t="str">
         <f>IF(组合逻辑真值表!Q12=1,$M11&amp;"+","")</f>
@@ -3293,11 +3439,11 @@
       </c>
       <c r="S11" s="4" t="str">
         <f>IF(组合逻辑真值表!R12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T11" s="4" t="str">
         <f>IF(组合逻辑真值表!S12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U11" s="4" t="str">
         <f>IF(组合逻辑真值表!T12=1,$M11&amp;"+","")</f>
@@ -3375,23 +3521,23 @@
       </c>
       <c r="N12" s="4" t="str">
         <f>IF(组合逻辑真值表!M13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O12" s="4" t="str">
         <f>IF(组合逻辑真值表!N13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P12" s="4" t="str">
         <f>IF(组合逻辑真值表!O13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q12" s="4" t="str">
         <f>IF(组合逻辑真值表!P13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="R12" s="4" t="str">
         <f>IF(组合逻辑真值表!Q13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S12" s="4" t="str">
         <f>IF(组合逻辑真值表!R13=1,$M12&amp;"+","")</f>
@@ -3399,7 +3545,7 @@
       </c>
       <c r="T12" s="4" t="str">
         <f>IF(组合逻辑真值表!S13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U12" s="4" t="str">
         <f>IF(组合逻辑真值表!T13=1,$M12&amp;"+","")</f>
@@ -3477,11 +3623,11 @@
       </c>
       <c r="N13" s="4" t="str">
         <f>IF(组合逻辑真值表!M14=1,$M13&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O13" s="4" t="str">
         <f>IF(组合逻辑真值表!N14=1,$M13&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P13" s="4" t="str">
         <f>IF(组合逻辑真值表!O14=1,$M13&amp;"+","")</f>
@@ -3493,15 +3639,15 @@
       </c>
       <c r="R13" s="4" t="str">
         <f>IF(组合逻辑真值表!Q14=1,$M13&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S13" s="4" t="str">
         <f>IF(组合逻辑真值表!R14=1,$M13&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T13" s="4" t="str">
         <f>IF(组合逻辑真值表!S14=1,$M13&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U13" s="4" t="str">
         <f>IF(组合逻辑真值表!T14=1,$M13&amp;"+","")</f>
@@ -3583,11 +3729,11 @@
       </c>
       <c r="O14" s="4" t="str">
         <f>IF(组合逻辑真值表!N15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P14" s="4" t="str">
         <f>IF(组合逻辑真值表!O15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q14" s="4" t="str">
         <f>IF(组合逻辑真值表!P15=1,$M14&amp;"+","")</f>
@@ -3595,11 +3741,11 @@
       </c>
       <c r="R14" s="4" t="str">
         <f>IF(组合逻辑真值表!Q15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S14" s="4" t="str">
         <f>IF(组合逻辑真值表!R15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T14" s="4" t="str">
         <f>IF(组合逻辑真值表!S15=1,$M14&amp;"+","")</f>
@@ -3681,7 +3827,7 @@
       </c>
       <c r="N15" s="4" t="str">
         <f>IF(组合逻辑真值表!M16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O15" s="4" t="str">
         <f>IF(组合逻辑真值表!N16=1,$M15&amp;"+","")</f>
@@ -3693,19 +3839,19 @@
       </c>
       <c r="Q15" s="4" t="str">
         <f>IF(组合逻辑真值表!P16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="R15" s="4" t="str">
         <f>IF(组合逻辑真值表!Q16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S15" s="4" t="str">
         <f>IF(组合逻辑真值表!R16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T15" s="4" t="str">
         <f>IF(组合逻辑真值表!S16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="U15" s="4" t="str">
         <f>IF(组合逻辑真值表!T16=1,$M15&amp;"+","")</f>
@@ -3783,15 +3929,15 @@
       </c>
       <c r="N16" s="4" t="str">
         <f>IF(组合逻辑真值表!M17=1,$M16&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O16" s="4" t="str">
         <f>IF(组合逻辑真值表!N17=1,$M16&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P16" s="4" t="str">
         <f>IF(组合逻辑真值表!O17=1,$M16&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q16" s="4" t="str">
         <f>IF(组合逻辑真值表!P17=1,$M16&amp;"+","")</f>
@@ -3799,11 +3945,11 @@
       </c>
       <c r="R16" s="4" t="str">
         <f>IF(组合逻辑真值表!Q17=1,$M16&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S16" s="4" t="str">
         <f>IF(组合逻辑真值表!R17=1,$M16&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="T16" s="4" t="str">
         <f>IF(组合逻辑真值表!S17=1,$M16&amp;"+","")</f>
@@ -3885,15 +4031,15 @@
       </c>
       <c r="N17" s="4" t="str">
         <f>IF(组合逻辑真值表!M18=1,$M17&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="O17" s="4" t="str">
         <f>IF(组合逻辑真值表!N18=1,$M17&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="P17" s="4" t="str">
         <f>IF(组合逻辑真值表!O18=1,$M17&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="Q17" s="4" t="str">
         <f>IF(组合逻辑真值表!P18=1,$M17&amp;"+","")</f>
@@ -3901,7 +4047,7 @@
       </c>
       <c r="R17" s="4" t="str">
         <f>IF(组合逻辑真值表!Q18=1,$M17&amp;"+","")</f>
-        <v/>
+        <v>+</v>
       </c>
       <c r="S17" s="4" t="str">
         <f>IF(组合逻辑真值表!R18=1,$M17&amp;"+","")</f>
@@ -5144,31 +5290,31 @@
       <c r="M31" s="37"/>
       <c r="N31" s="5" t="str">
         <f t="shared" ref="N31:O31" si="2">IF(LEN(N32)&gt;1,LEFT(N32,LEN(N32)-1),"")</f>
-        <v>In5+In3&amp;~In4&amp;~In5+In1&amp;~In2&amp;~In3&amp;~In4&amp;~In5</v>
+        <v>In3&amp;~In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4+++++++++</v>
       </c>
       <c r="O31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>In3&amp;~In4&amp;~In5+In2&amp;~In3&amp;~In4&amp;~In5</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4+++++++++</v>
       </c>
       <c r="P31" s="5" t="str">
         <f t="shared" ref="P31" si="3">IF(LEN(P32)&gt;1,LEFT(P32,LEN(P32)-1),"")</f>
-        <v>In5+In4&amp;~In5</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4+In2&amp;~In3&amp;~In4+++++++++</v>
       </c>
       <c r="Q31" s="5" t="str">
         <f t="shared" ref="Q31" si="4">IF(LEN(Q32)&gt;1,LEFT(Q32,LEN(Q32)-1),"")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+~In1&amp;~In2&amp;~In3&amp;In4+In3&amp;~In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4+++++</v>
       </c>
       <c r="R31" s="5" t="str">
         <f t="shared" ref="R31" si="5">IF(LEN(R32)&gt;1,LEFT(R32,LEN(R32)-1),"")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4++++++++</v>
       </c>
       <c r="S31" s="5" t="str">
         <f t="shared" ref="S31" si="6">IF(LEN(S32)&gt;1,LEFT(S32,LEN(S32)-1),"")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4+In2&amp;~In3&amp;~In4++++++++</v>
       </c>
       <c r="T31" s="5" t="str">
         <f t="shared" ref="T31" si="7">IF(LEN(T32)&gt;1,LEFT(T32,LEN(T32)-1),"")</f>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+~In1&amp;~In2&amp;~In3&amp;In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4++++++++</v>
       </c>
       <c r="U31" s="5" t="str">
         <f t="shared" ref="U31" si="8">IF(LEN(U32)&gt;1,LEFT(U32,LEN(U32)-1),"")</f>
@@ -5207,31 +5353,31 @@
       <c r="M32" s="6"/>
       <c r="N32" s="7" t="str">
         <f>CONCATENATE(N2,N3,N4,N5,N6,N7,N8,N9,N10,N11,N12,N13,N14,N15,N16,N17,N18,N19,N20,N21,N22,N23,N24,N25,N26,N27,N28,N29,N30)</f>
-        <v>In5+In3&amp;~In4&amp;~In5+In1&amp;~In2&amp;~In3&amp;~In4&amp;~In5+</v>
+        <v>In3&amp;~In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4++++++++++</v>
       </c>
       <c r="O32" s="7" t="str">
         <f t="shared" ref="O32:Y32" si="13">CONCATENATE(O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30)</f>
-        <v>In3&amp;~In4&amp;~In5+In2&amp;~In3&amp;~In4&amp;~In5+</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4++++++++++</v>
       </c>
       <c r="P32" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>In5+In4&amp;~In5+</v>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4+In2&amp;~In3&amp;~In4++++++++++</v>
       </c>
       <c r="Q32" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+~In1&amp;~In2&amp;~In3&amp;In4+In3&amp;~In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4++++++</v>
       </c>
       <c r="R32" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4+++++++++</v>
       </c>
       <c r="S32" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+In3&amp;~In4+In2&amp;~In3&amp;~In4+++++++++</v>
       </c>
       <c r="T32" s="7" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>~In1&amp;~In2&amp;~In3&amp;~In4+~In1&amp;~In2&amp;~In3&amp;In4+In2&amp;~In3&amp;~In4+In1&amp;~In2&amp;~In3&amp;~In4+++++++++</v>
       </c>
       <c r="U32" s="7" t="str">
         <f t="shared" si="13"/>

</xml_diff>